<commit_message>
Inicio, como le hago con las mamadas del enunciado :( puta claudia
</commit_message>
<xml_diff>
--- a/Alohandes/data/Modelos/Esquema BD.xlsx
+++ b/Alohandes/data/Modelos/Esquema BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECLIPSE\HotelManagement\Alohandes\data\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC15C201-A4DC-45D7-848B-FA87012C24EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40E1D5A-2DC7-43ED-A61F-2D0793A9CA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EEF67A9-6324-49A2-AA74-E29D07B2AB68}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Relacional" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -450,6 +449,77 @@
   </si>
   <si>
     <r>
+      <t>FK.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>OPERADOR.ID, NN</t>
+    </r>
+  </si>
+  <si>
+    <t>MENAJE</t>
+  </si>
+  <si>
+    <t>HABILITADA</t>
+  </si>
+  <si>
+    <t>FECHA_REALIZACION</t>
+  </si>
+  <si>
+    <t>COLECTIVA</t>
+  </si>
+  <si>
+    <t>RESERVA_COLECTIVA</t>
+  </si>
+  <si>
+    <r>
+      <t>NN, FK.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>OFERTA.ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NN, FK.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>CLIENTE.ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Tw Cen MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>RESERVA_COLECTIVA.ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>NN, CK</t>
     </r>
     <r>
@@ -459,78 +529,7 @@
         <rFont val="Tw Cen MT"/>
         <family val="2"/>
       </rPr>
-      <t>(HOTELERIA, PERSONA_NATURAL, )</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>FK.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>OPERADOR.ID, NN</t>
-    </r>
-  </si>
-  <si>
-    <t>MENAJE</t>
-  </si>
-  <si>
-    <t>HABILITADA</t>
-  </si>
-  <si>
-    <t>FECHA_REALIZACION</t>
-  </si>
-  <si>
-    <t>COLECTIVA</t>
-  </si>
-  <si>
-    <t>RESERVA_COLECTIVA</t>
-  </si>
-  <si>
-    <r>
-      <t>NN, FK.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>OFERTA.ID</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>NN, FK.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>CLIENTE.ID</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>FK.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Tw Cen MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>RESERVA_COLECTIVA.ID</t>
+      <t>(HOTELERIA, PERSONA_NATURAL, VIVIENDA_UNIVERSITARIA)</t>
     </r>
   </si>
 </sst>
@@ -1028,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE441C97-7F2D-4289-AB1E-C697E71C467D}">
   <dimension ref="B2:CN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="CK7" sqref="CK7:CN10"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="AN15" sqref="AN15:AN16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,12 +1037,12 @@
     <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="33.6640625" customWidth="1"/>
@@ -1055,7 +1054,7 @@
     <col min="25" max="25" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
@@ -1118,6 +1117,13 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
+      <c r="I2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
       <c r="O2" s="10" t="s">
         <v>56</v>
       </c>
@@ -1176,6 +1182,21 @@
       <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1204,7 +1225,7 @@
         <v>73</v>
       </c>
       <c r="AS3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>5</v>
@@ -1258,7 +1279,7 @@
         <v>49</v>
       </c>
       <c r="CI3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:92" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1279,6 +1300,21 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>6</v>
@@ -1383,6 +1419,21 @@
       </c>
       <c r="G5" s="6" t="s">
         <v>55</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>57</v>
@@ -1465,23 +1516,16 @@
         <v>42</v>
       </c>
       <c r="CG5" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="CH5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="CH5" s="7" t="s">
+      <c r="CI5" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="CI5" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:92" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
       <c r="S7" s="10" t="s">
         <v>61</v>
       </c>
@@ -1532,28 +1576,13 @@
       <c r="BY7" s="11"/>
       <c r="BZ7" s="11"/>
       <c r="CK7" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CL7" s="10"/>
       <c r="CM7" s="10"/>
       <c r="CN7" s="10"/>
     </row>
     <row r="8" spans="2:92" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="S8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1639,7 +1668,7 @@
         <v>19</v>
       </c>
       <c r="BU8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BW8" s="1" t="s">
         <v>5</v>
@@ -1657,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="CL8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="CM8" s="2" t="s">
         <v>67</v>
@@ -1667,21 +1696,6 @@
       </c>
     </row>
     <row r="9" spans="2:92" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="I9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="S9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1795,21 +1809,6 @@
       </c>
     </row>
     <row r="10" spans="2:92" x14ac:dyDescent="0.3">
-      <c r="I10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="S10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AD10" s="5" t="s">
         <v>2</v>
@@ -1927,7 +1926,7 @@
     <mergeCell ref="CK7:CN7"/>
     <mergeCell ref="CB2:CI2"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="I2:M2"/>
     <mergeCell ref="BJ2:BO2"/>
     <mergeCell ref="BD7:BH7"/>
     <mergeCell ref="AY2:BB2"/>

</xml_diff>